<commit_message>
include .env in the repo
Only info for demo purposes included
</commit_message>
<xml_diff>
--- a/data/daily_runoff/12176_Sihl_example_river_runoff.xlsx
+++ b/data/daily_runoff/12176_Sihl_example_river_runoff.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10114"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A72176A5-BDCA-B648-9979-753128EF4A68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{958CDAAA-9E5D-1848-8FD8-0B8952C202B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="760" windowWidth="17120" windowHeight="17660" tabRatio="841" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38181,8 +38181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B366"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A274" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B306" sqref="B306"/>
+    <sheetView tabSelected="1" topLeftCell="A334" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B356" sqref="B356"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -40634,301 +40634,401 @@
       <c r="A306" s="5">
         <v>37926</v>
       </c>
-      <c r="B306" s="6"/>
+      <c r="B306" s="6">
+        <v>14.1</v>
+      </c>
     </row>
     <row r="307" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A307" s="5">
         <v>37927</v>
       </c>
-      <c r="B307" s="6"/>
+      <c r="B307" s="6">
+        <v>7.9</v>
+      </c>
     </row>
     <row r="308" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A308" s="5">
         <v>37928</v>
       </c>
-      <c r="B308" s="6"/>
+      <c r="B308" s="6">
+        <v>5.55</v>
+      </c>
     </row>
     <row r="309" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A309" s="5">
         <v>37929</v>
       </c>
-      <c r="B309" s="6"/>
+      <c r="B309" s="6">
+        <v>4.09</v>
+      </c>
     </row>
     <row r="310" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A310" s="5">
         <v>37930</v>
       </c>
-      <c r="B310" s="6"/>
+      <c r="B310" s="6">
+        <v>3.18</v>
+      </c>
     </row>
     <row r="311" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A311" s="5">
         <v>37931</v>
       </c>
-      <c r="B311" s="6"/>
+      <c r="B311" s="6">
+        <v>3.05</v>
+      </c>
     </row>
     <row r="312" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A312" s="5">
         <v>37932</v>
       </c>
-      <c r="B312" s="6"/>
+      <c r="B312" s="6">
+        <v>3.08</v>
+      </c>
     </row>
     <row r="313" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A313" s="5">
         <v>37933</v>
       </c>
-      <c r="B313" s="6"/>
+      <c r="B313" s="6">
+        <v>3.01</v>
+      </c>
     </row>
     <row r="314" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A314" s="5">
         <v>37934</v>
       </c>
-      <c r="B314" s="6"/>
+      <c r="B314" s="6">
+        <v>2.92</v>
+      </c>
     </row>
     <row r="315" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A315" s="5">
         <v>37935</v>
       </c>
-      <c r="B315" s="6"/>
+      <c r="B315" s="6">
+        <v>2.89</v>
+      </c>
     </row>
     <row r="316" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A316" s="5">
         <v>37936</v>
       </c>
-      <c r="B316" s="6"/>
+      <c r="B316" s="6">
+        <v>2.86</v>
+      </c>
     </row>
     <row r="317" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A317" s="5">
         <v>37937</v>
       </c>
-      <c r="B317" s="6"/>
+      <c r="B317" s="6">
+        <v>2.86</v>
+      </c>
     </row>
     <row r="318" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A318" s="5">
         <v>37938</v>
       </c>
-      <c r="B318" s="6"/>
+      <c r="B318" s="6">
+        <v>10.3</v>
+      </c>
     </row>
     <row r="319" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A319" s="5">
         <v>37939</v>
       </c>
-      <c r="B319" s="6"/>
+      <c r="B319" s="6">
+        <v>7.5</v>
+      </c>
     </row>
     <row r="320" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A320" s="5">
         <v>37940</v>
       </c>
-      <c r="B320" s="6"/>
+      <c r="B320" s="6">
+        <v>3.77</v>
+      </c>
     </row>
     <row r="321" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A321" s="5">
         <v>37941</v>
       </c>
-      <c r="B321" s="6"/>
+      <c r="B321" s="6">
+        <v>3.31</v>
+      </c>
     </row>
     <row r="322" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A322" s="5">
         <v>37942</v>
       </c>
-      <c r="B322" s="6"/>
+      <c r="B322" s="6">
+        <v>6.58</v>
+      </c>
     </row>
     <row r="323" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A323" s="5">
         <v>37943</v>
       </c>
-      <c r="B323" s="6"/>
+      <c r="B323" s="6">
+        <v>5.45</v>
+      </c>
     </row>
     <row r="324" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A324" s="5">
         <v>37944</v>
       </c>
-      <c r="B324" s="6"/>
+      <c r="B324" s="6">
+        <v>3.73</v>
+      </c>
     </row>
     <row r="325" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A325" s="5">
         <v>37945</v>
       </c>
-      <c r="B325" s="6"/>
+      <c r="B325" s="6">
+        <v>3.15</v>
+      </c>
     </row>
     <row r="326" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A326" s="5">
         <v>37946</v>
       </c>
-      <c r="B326" s="6"/>
+      <c r="B326" s="6">
+        <v>3.05</v>
+      </c>
     </row>
     <row r="327" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A327" s="5">
         <v>37947</v>
       </c>
-      <c r="B327" s="6"/>
+      <c r="B327" s="6">
+        <v>2.91</v>
+      </c>
     </row>
     <row r="328" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A328" s="5">
         <v>37948</v>
       </c>
-      <c r="B328" s="6"/>
+      <c r="B328" s="6">
+        <v>2.9</v>
+      </c>
     </row>
     <row r="329" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A329" s="5">
         <v>37949</v>
       </c>
-      <c r="B329" s="6"/>
+      <c r="B329" s="6">
+        <v>2.84</v>
+      </c>
     </row>
     <row r="330" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A330" s="5">
         <v>37950</v>
       </c>
-      <c r="B330" s="6"/>
+      <c r="B330" s="6">
+        <v>2.83</v>
+      </c>
     </row>
     <row r="331" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A331" s="5">
         <v>37951</v>
       </c>
-      <c r="B331" s="6"/>
+      <c r="B331" s="6">
+        <v>2.77</v>
+      </c>
     </row>
     <row r="332" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A332" s="5">
         <v>37952</v>
       </c>
-      <c r="B332" s="6"/>
+      <c r="B332" s="6">
+        <v>2.87</v>
+      </c>
     </row>
     <row r="333" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A333" s="5">
         <v>37953</v>
       </c>
-      <c r="B333" s="6"/>
+      <c r="B333" s="6">
+        <v>6.3</v>
+      </c>
     </row>
     <row r="334" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A334" s="5">
         <v>37954</v>
       </c>
-      <c r="B334" s="6"/>
+      <c r="B334" s="6">
+        <v>5.79</v>
+      </c>
     </row>
     <row r="335" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A335" s="5">
         <v>37955</v>
       </c>
-      <c r="B335" s="6"/>
+      <c r="B335" s="6">
+        <v>4.38</v>
+      </c>
     </row>
     <row r="336" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A336" s="5">
         <v>37956</v>
       </c>
-      <c r="B336" s="6"/>
+      <c r="B336" s="6">
+        <v>4.8499999999999996</v>
+      </c>
     </row>
     <row r="337" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A337" s="5">
         <v>37957</v>
       </c>
-      <c r="B337" s="6"/>
+      <c r="B337" s="6">
+        <v>8.1999999999999993</v>
+      </c>
     </row>
     <row r="338" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A338" s="5">
         <v>37958</v>
       </c>
-      <c r="B338" s="6"/>
+      <c r="B338" s="6">
+        <v>6.09</v>
+      </c>
     </row>
     <row r="339" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A339" s="5">
         <v>37959</v>
       </c>
-      <c r="B339" s="6"/>
+      <c r="B339" s="6">
+        <v>3.86</v>
+      </c>
     </row>
     <row r="340" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A340" s="5">
         <v>37960</v>
       </c>
-      <c r="B340" s="6"/>
+      <c r="B340" s="6">
+        <v>3.28</v>
+      </c>
     </row>
     <row r="341" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A341" s="5">
         <v>37961</v>
       </c>
-      <c r="B341" s="6"/>
+      <c r="B341" s="6">
+        <v>3.09</v>
+      </c>
     </row>
     <row r="342" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A342" s="5">
         <v>37962</v>
       </c>
-      <c r="B342" s="6"/>
+      <c r="B342" s="6">
+        <v>3.06</v>
+      </c>
     </row>
     <row r="343" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A343" s="5">
         <v>37963</v>
       </c>
-      <c r="B343" s="6"/>
+      <c r="B343" s="6">
+        <v>2.98</v>
+      </c>
     </row>
     <row r="344" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A344" s="5">
         <v>37964</v>
       </c>
-      <c r="B344" s="6"/>
+      <c r="B344" s="6">
+        <v>2.9</v>
+      </c>
     </row>
     <row r="345" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A345" s="5">
         <v>37965</v>
       </c>
-      <c r="B345" s="6"/>
+      <c r="B345" s="6">
+        <v>2.88</v>
+      </c>
     </row>
     <row r="346" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A346" s="5">
         <v>37966</v>
       </c>
-      <c r="B346" s="6"/>
+      <c r="B346" s="6">
+        <v>2.85</v>
+      </c>
     </row>
     <row r="347" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A347" s="5">
         <v>37967</v>
       </c>
-      <c r="B347" s="6"/>
+      <c r="B347" s="6">
+        <v>2.86</v>
+      </c>
     </row>
     <row r="348" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A348" s="5">
         <v>37968</v>
       </c>
-      <c r="B348" s="6"/>
+      <c r="B348" s="6">
+        <v>2.8</v>
+      </c>
     </row>
     <row r="349" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A349" s="5">
         <v>37969</v>
       </c>
-      <c r="B349" s="6"/>
+      <c r="B349" s="6">
+        <v>3.33</v>
+      </c>
     </row>
     <row r="350" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A350" s="5">
         <v>37970</v>
       </c>
-      <c r="B350" s="6"/>
+      <c r="B350" s="6">
+        <v>4.95</v>
+      </c>
     </row>
     <row r="351" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A351" s="5">
         <v>37971</v>
       </c>
-      <c r="B351" s="6"/>
+      <c r="B351" s="6">
+        <v>2.99</v>
+      </c>
     </row>
     <row r="352" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A352" s="5">
         <v>37972</v>
       </c>
-      <c r="B352" s="6"/>
+      <c r="B352" s="6">
+        <v>2.89</v>
+      </c>
     </row>
     <row r="353" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A353" s="5">
         <v>37973</v>
       </c>
-      <c r="B353" s="6"/>
+      <c r="B353" s="6">
+        <v>2.79</v>
+      </c>
     </row>
     <row r="354" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A354" s="5">
         <v>37974</v>
       </c>
-      <c r="B354" s="6"/>
+      <c r="B354" s="6">
+        <v>2.79</v>
+      </c>
     </row>
     <row r="355" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A355" s="5">
         <v>37975</v>
       </c>
-      <c r="B355" s="6"/>
+      <c r="B355" s="6">
+        <v>2.8</v>
+      </c>
     </row>
     <row r="356" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A356" s="5">

</xml_diff>

<commit_message>
first steps towards dockerization
</commit_message>
<xml_diff>
--- a/data/daily_runoff/12176_Sihl_example_river_runoff.xlsx
+++ b/data/daily_runoff/12176_Sihl_example_river_runoff.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10114"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{958CDAAA-9E5D-1848-8FD8-0B8952C202B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{438CB051-C545-4440-86B6-235F5F39F774}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="760" windowWidth="17120" windowHeight="17660" tabRatio="841" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13120" yWindow="760" windowWidth="17120" windowHeight="17660" tabRatio="841" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2000" sheetId="9" r:id="rId1"/>
@@ -38181,8 +38181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B366"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A334" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B356" sqref="B356"/>
+    <sheetView topLeftCell="A341" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B357" sqref="B357"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -41034,67 +41034,89 @@
       <c r="A356" s="5">
         <v>37976</v>
       </c>
-      <c r="B356" s="6"/>
+      <c r="B356" s="6">
+        <v>3.75</v>
+      </c>
     </row>
     <row r="357" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A357" s="5">
         <v>37977</v>
       </c>
-      <c r="B357" s="6"/>
+      <c r="B357" s="6">
+        <v>6.57</v>
+      </c>
     </row>
     <row r="358" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A358" s="5">
         <v>37978</v>
       </c>
-      <c r="B358" s="6"/>
+      <c r="B358" s="6">
+        <v>3.16</v>
+      </c>
     </row>
     <row r="359" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A359" s="5">
         <v>37979</v>
       </c>
-      <c r="B359" s="6"/>
+      <c r="B359" s="6">
+        <v>2.73</v>
+      </c>
     </row>
     <row r="360" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A360" s="5">
         <v>37980</v>
       </c>
-      <c r="B360" s="6"/>
+      <c r="B360" s="6">
+        <v>2.17</v>
+      </c>
     </row>
     <row r="361" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A361" s="5">
         <v>37981</v>
       </c>
-      <c r="B361" s="6"/>
+      <c r="B361" s="6">
+        <v>2.67</v>
+      </c>
     </row>
     <row r="362" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A362" s="5">
         <v>37982</v>
       </c>
-      <c r="B362" s="6"/>
+      <c r="B362" s="6">
+        <v>3.15</v>
+      </c>
     </row>
     <row r="363" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A363" s="5">
         <v>37983</v>
       </c>
-      <c r="B363" s="6"/>
+      <c r="B363" s="6">
+        <v>3.23</v>
+      </c>
     </row>
     <row r="364" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A364" s="5">
         <v>37984</v>
       </c>
-      <c r="B364" s="6"/>
+      <c r="B364" s="6">
+        <v>3.73</v>
+      </c>
     </row>
     <row r="365" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A365" s="5">
         <v>37985</v>
       </c>
-      <c r="B365" s="6"/>
+      <c r="B365" s="6">
+        <v>3.21</v>
+      </c>
     </row>
     <row r="366" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A366" s="5">
         <v>37986</v>
       </c>
-      <c r="B366" s="6"/>
+      <c r="B366" s="6">
+        <v>3.04</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -41106,8 +41128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F367"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -41128,32 +41150,42 @@
       <c r="A2" s="5">
         <v>37987</v>
       </c>
-      <c r="B2" s="6"/>
+      <c r="B2" s="6">
+        <v>2.88</v>
+      </c>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>37988</v>
       </c>
-      <c r="B3" s="6"/>
+      <c r="B3" s="6">
+        <v>2.9</v>
+      </c>
     </row>
     <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>37989</v>
       </c>
-      <c r="B4" s="6"/>
+      <c r="B4" s="6">
+        <v>2.8</v>
+      </c>
     </row>
     <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>37990</v>
       </c>
-      <c r="B5" s="6"/>
+      <c r="B5" s="6">
+        <v>2.85</v>
+      </c>
     </row>
     <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>37991</v>
       </c>
-      <c r="B6" s="6"/>
+      <c r="B6" s="6">
+        <v>2.78</v>
+      </c>
     </row>
     <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="5">

</xml_diff>